<commit_message>
preliminary stats finished ...
</commit_message>
<xml_diff>
--- a/tabs/pd_cogREH_desc.xlsx
+++ b/tabs/pd_cogREH_desc.xlsx
@@ -22,22 +22,22 @@
     <t xml:space="preserve"/>
   </si>
   <si>
-    <t xml:space="preserve">EXP_baseline</t>
+    <t xml:space="preserve">EXP_1baseline</t>
   </si>
   <si>
-    <t xml:space="preserve">EXP_retest</t>
+    <t xml:space="preserve">EXP_2retest</t>
   </si>
   <si>
-    <t xml:space="preserve">EXP_follow-up</t>
+    <t xml:space="preserve">EXP_3followup</t>
   </si>
   <si>
-    <t xml:space="preserve">CON_baseline</t>
+    <t xml:space="preserve">CON_1baseline</t>
   </si>
   <si>
-    <t xml:space="preserve">CON_retest</t>
+    <t xml:space="preserve">CON_2retest</t>
   </si>
   <si>
-    <t xml:space="preserve">CON_follow-up</t>
+    <t xml:space="preserve">CON_3followup</t>
   </si>
   <si>
     <t xml:space="preserve">Gender</t>

</xml_diff>